<commit_message>
Actualiza archivos de carga de lotes bdb
</commit_message>
<xml_diff>
--- a/build/assets/statics/bdb/DESBLOQUEO TARJETAS.xlsx
+++ b/build/assets/statics/bdb/DESBLOQUEO TARJETAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squijano\Desktop\BANCO DE BOGOTA\ARCHIVOS AUTOGESTION CEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923BA2F1-171A-4669-ADAC-4BF406E26767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A738A17-B2E6-481A-8016-9E3D1FC68665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="473" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>TIPO REGISTRO</t>
   </si>
@@ -240,9 +240,6 @@
     <t xml:space="preserve">No se debe alterar el formato del archivo ya que esto afectará la carga del mismo en el portal Corporativo. </t>
   </si>
   <si>
-    <t>En la fila 8 se debe indicar cuántas tarjetas serán procesadas en este archivo, así como la fecha de cargue del mismo.</t>
-  </si>
-  <si>
     <t>Este formato permite desbloquear la tarjeta de uno o más tarjetahabientes desde el portal Corporativo de Tarjetas Prepago.</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>Los títulos de cada columna contienen una Nota, la cual describe el dato a ingresar en cada una de ellas.</t>
+  </si>
+  <si>
+    <t>En la fila 8 del archivo se debe indicar cuántas tarjetas serán procesadas en este archivo, así como la fecha de cargue del mismo.</t>
+  </si>
+  <si>
+    <t>Desde la fila 11 del archivo se deben agregar el listado de tarjetas a desbloquear. No debe dejar filas vacías. La fila vacía indica fin de archivo.</t>
   </si>
 </sst>
 </file>
@@ -631,6 +634,13 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -651,13 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1252,12 +1255,12 @@
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1267,7 +1270,7 @@
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="11"/>
       <c r="D3" s="14"/>
       <c r="E3" s="12"/>
@@ -1287,7 +1290,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
@@ -1301,19 +1304,19 @@
     <row r="5" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9"/>
       <c r="C5" s="6"/>
-      <c r="F5" s="8" t="s">
-        <v>18</v>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
       <c r="F6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -1327,8 +1330,8 @@
       <c r="C7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="I7" s="6"/>
     </row>
@@ -1340,23 +1343,26 @@
         <v>1</v>
       </c>
       <c r="C8" s="30"/>
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="44" t="s">
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="45"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:14" s="7" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1392,8 +1398,8 @@
         <v>9</v>
       </c>
       <c r="B11" s="38"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="F11" s="32"/>
       <c r="G11" s="38"/>
       <c r="H11" s="32"/>
@@ -6896,7 +6902,7 @@
       <c r="H511" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/MXmFFC9SinSGBxxzUY+x1c2SZfE/DAzeTrI2fwmPcPK7I1LUnqfVh3AsYOMK34ni5y2iQVzgacNFnoWypKfxQ==" saltValue="4/Spja5KmjvS4otzJmci6A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bu5TtnuQMpndLXN1JfSMG0tZJE2wTpa/+Vw73W1BSRE1j2rgjbpglaBPNiJeZ9NNsCxZw/9pfhmZa5lNJxLW1g==" saltValue="WidMmd6KCa2s7OVNI5UrVw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" deleteRows="0"/>
   <protectedRanges>
     <protectedRange sqref="B11:B510" name="Rango1_1_1_1_1"/>
     <protectedRange sqref="A8:C8" name="Rango1_1_1"/>

</xml_diff>